<commit_message>
add recursion solution for lc.24
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,6 +185,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,7 +470,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,7 +536,7 @@
       <c r="A5" s="5">
         <v>43756</v>
       </c>
-      <c r="B5" s="8" t="str">
+      <c r="B5" s="9" t="str">
         <f>Sheet2!B5</f>
         <v>25,239</v>
       </c>
@@ -547,7 +550,7 @@
       <c r="A6" s="5">
         <v>43757</v>
       </c>
-      <c r="B6" s="8" t="str">
+      <c r="B6" s="9" t="str">
         <f>Sheet2!B6</f>
         <v>155,641</v>
       </c>
@@ -561,7 +564,7 @@
       <c r="A7" s="5">
         <v>43758</v>
       </c>
-      <c r="B7" s="8" t="str">
+      <c r="B7" s="9" t="str">
         <f>Sheet2!B7</f>
         <v>20,42,84</v>
       </c>

</xml_diff>

<commit_message>
add lc.155, lc.641 passed with use of list.List in golang
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -150,7 +150,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,10 +184,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +497,7 @@
       <c r="A2" s="5">
         <v>43753</v>
       </c>
-      <c r="B2" s="8" t="str">
+      <c r="B2" s="9" t="str">
         <f>Sheet2!B2</f>
         <v>283,11</v>
       </c>
@@ -508,11 +508,11 @@
       <c r="A3" s="5">
         <v>43754</v>
       </c>
-      <c r="B3" s="8" t="str">
+      <c r="B3" s="9" t="str">
         <f>Sheet2!B3</f>
         <v>70,15,66,88</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="9" t="str">
         <f>Sheet2!B2</f>
         <v>283,11</v>
       </c>
@@ -522,11 +522,11 @@
       <c r="A4" s="5">
         <v>43755</v>
       </c>
-      <c r="B4" s="8" t="str">
+      <c r="B4" s="9" t="str">
         <f>Sheet2!B4</f>
         <v>24,206,141,142</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="9" t="str">
         <f>Sheet2!B3</f>
         <v>70,15,66,88</v>
       </c>
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" s="9" t="str">
         <f>Sheet2!B5</f>
-        <v>25,239</v>
+        <v>155,641</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>Sheet2!B4</f>
@@ -550,13 +550,13 @@
       <c r="A6" s="5">
         <v>43757</v>
       </c>
-      <c r="B6" s="9" t="str">
+      <c r="B6" s="8" t="str">
         <f>Sheet2!B6</f>
-        <v>155,641</v>
+        <v>25,239</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>Sheet2!B5</f>
-        <v>25,239</v>
+        <v>155,641</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -564,13 +564,13 @@
       <c r="A7" s="5">
         <v>43758</v>
       </c>
-      <c r="B7" s="9" t="str">
+      <c r="B7" s="8" t="str">
         <f>Sheet2!B7</f>
         <v>20,42,84</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>Sheet2!B6</f>
-        <v>155,641</v>
+        <v>25,239</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="D13" s="3" t="str">
         <f>Sheet2!B5</f>
-        <v>25,239</v>
+        <v>155,641</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -684,7 +684,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>Sheet2!B6</f>
-        <v>155,641</v>
+        <v>25,239</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1005,7 +1005,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1043,7 @@
         <v>43756</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1051,7 +1051,7 @@
         <v>43757</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1"/>
     </row>

</xml_diff>

<commit_message>
add lc.42, more understanding required
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-18700" yWindow="460" windowWidth="18700" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>283,11</t>
   </si>
   <si>
-    <t>20,42,84</t>
-  </si>
-  <si>
     <t>70,15,66,88</t>
   </si>
   <si>
@@ -117,7 +114,10 @@
     <t>24,206,141,142</t>
   </si>
   <si>
-    <t>25,239</t>
+    <t>42</t>
+  </si>
+  <si>
+    <t>20,84,25,239</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,7 +540,7 @@
         <f>Sheet2!B5</f>
         <v>155,641</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="9" t="str">
         <f>Sheet2!B4</f>
         <v>24,206,141,142</v>
       </c>
@@ -550,9 +550,9 @@
       <c r="A6" s="5">
         <v>43757</v>
       </c>
-      <c r="B6" s="8" t="str">
+      <c r="B6" s="9" t="str">
         <f>Sheet2!B6</f>
-        <v>25,239</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>Sheet2!B5</f>
@@ -566,11 +566,11 @@
       </c>
       <c r="B7" s="8" t="str">
         <f>Sheet2!B7</f>
-        <v>20,42,84</v>
+        <v>20,84,25,239</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>Sheet2!B6</f>
-        <v>25,239</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="C8" s="3" t="str">
         <f>Sheet2!B7</f>
-        <v>20,42,84</v>
+        <v>20,84,25,239</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f>Sheet2!B6</f>
-        <v>25,239</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -701,7 +701,7 @@
       </c>
       <c r="D15" s="3" t="str">
         <f>Sheet2!B7</f>
-        <v>20,42,84</v>
+        <v>20,84,25,239</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1027,7 @@
         <v>43754</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>43755</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1043,7 +1043,7 @@
         <v>43756</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1051,7 +1051,7 @@
         <v>43757</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1060,7 +1060,7 @@
         <v>43758</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add some big O images
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-18700" yWindow="460" windowWidth="18700" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +561,7 @@
         <f>Sheet2!B6</f>
         <v>42</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="9" t="str">
         <f>Sheet2!B5</f>
         <v>20,155,641</v>
       </c>
@@ -1011,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add tree, add lc.94,144,145
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>242,49</t>
+  </si>
+  <si>
+    <t>94,144,145</t>
   </si>
 </sst>
 </file>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,9 +599,9 @@
       <c r="A9" s="5">
         <v>43760</v>
       </c>
-      <c r="B9" s="8" t="str">
+      <c r="B9" s="9" t="str">
         <f>Sheet2!B9</f>
-        <v>8</v>
+        <v>94,144,145</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>Sheet2!B8</f>
@@ -619,7 +619,7 @@
       </c>
       <c r="C10" s="3" t="str">
         <f>Sheet2!B9</f>
-        <v>8</v>
+        <v>94,144,145</v>
       </c>
       <c r="D10" s="3" t="str">
         <f>Sheet2!B2</f>
@@ -742,7 +742,7 @@
       </c>
       <c r="D17" s="3" t="str">
         <f>Sheet2!B9</f>
-        <v>8</v>
+        <v>94,144,145</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1011,8 +1011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1023,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1031,10 +1031,10 @@
         <v>43753</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,7 +1042,7 @@
         <v>43754</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
         <v>43755</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>43756</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1066,7 +1066,7 @@
         <v>43757</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
         <v>43758</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,7 +1082,7 @@
         <v>43759</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>43760</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,7 +1098,7 @@
         <v>43761</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>43762</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1114,7 +1114,7 @@
         <v>43763</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1122,7 +1122,7 @@
         <v>43764</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1130,7 +1130,7 @@
         <v>43765</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1138,7 +1138,7 @@
         <v>43766</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
         <v>43767</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
         <v>43768</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,7 +1162,7 @@
         <v>43769</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1170,7 +1170,7 @@
         <v>43770</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
         <v>43771</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>43772</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>43773</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1202,7 +1202,7 @@
         <v>43774</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>43775</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>43776</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1226,7 +1226,7 @@
         <v>43777</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>43778</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
         <v>43779</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,7 +1250,7 @@
         <v>43780</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1258,7 +1258,7 @@
         <v>43781</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,7 +1266,7 @@
         <v>43782</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add lc.104,111,226,297,98, only recursion is given and other solutions are required
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21440" yWindow="2400" windowWidth="27800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>9</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>10</t>
   </si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>94,144,145,589,590</t>
+  </si>
+  <si>
+    <t>297?</t>
+  </si>
+  <si>
+    <t>22,98,104,111,226</t>
   </si>
 </sst>
 </file>
@@ -477,15 +480,15 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -613,9 +616,9 @@
       <c r="A10" s="5">
         <v>43761</v>
       </c>
-      <c r="B10" s="8" t="str">
+      <c r="B10" s="9" t="str">
         <f>Sheet2!B10</f>
-        <v>9</v>
+        <v>22,98,104,111,226</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>Sheet2!B9</f>
@@ -636,7 +639,7 @@
       </c>
       <c r="C11" s="3" t="str">
         <f>Sheet2!B10</f>
-        <v>9</v>
+        <v>22,98,104,111,226</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>Sheet2!B3</f>
@@ -759,7 +762,7 @@
       </c>
       <c r="D18" s="3" t="str">
         <f>Sheet2!B10</f>
-        <v>9</v>
+        <v>22,98,104,111,226</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1012,18 +1015,18 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D1" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1031,10 +1034,10 @@
         <v>43753</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,7 +1045,10 @@
         <v>43754</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1050,7 +1056,7 @@
         <v>43755</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1058,7 +1064,7 @@
         <v>43756</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1066,7 +1072,7 @@
         <v>43757</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1074,7 +1080,7 @@
         <v>43758</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1082,7 +1088,7 @@
         <v>43759</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1090,7 +1096,7 @@
         <v>43760</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,7 +1104,7 @@
         <v>43761</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1106,7 +1112,7 @@
         <v>43762</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1114,7 +1120,7 @@
         <v>43763</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1122,7 +1128,7 @@
         <v>43764</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1130,7 +1136,7 @@
         <v>43765</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1138,7 +1144,7 @@
         <v>43766</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1146,7 +1152,7 @@
         <v>43767</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1154,7 +1160,7 @@
         <v>43768</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1162,7 +1168,7 @@
         <v>43769</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1170,7 +1176,7 @@
         <v>43770</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1178,7 +1184,7 @@
         <v>43771</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1186,7 +1192,7 @@
         <v>43772</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1194,7 +1200,7 @@
         <v>43773</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1202,7 +1208,7 @@
         <v>43774</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1210,7 +1216,7 @@
         <v>43775</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,7 +1224,7 @@
         <v>43776</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1226,7 +1232,7 @@
         <v>43777</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1234,7 +1240,7 @@
         <v>43778</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1242,7 +1248,7 @@
         <v>43779</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,7 +1256,7 @@
         <v>43780</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1258,7 +1264,7 @@
         <v>43781</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,7 +1272,7 @@
         <v>43782</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update readme, add day-by-day-timeline
</commit_message>
<xml_diff>
--- a/A.schedule.xlsx
+++ b/A.schedule.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>